<commit_message>
add HashMap and Tree category, and put related packages into them
</commit_message>
<xml_diff>
--- a/lc/resource/leetcode_category.xlsx
+++ b/lc/resource/leetcode_category.xlsx
@@ -4,19 +4,22 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="30" windowWidth="27795" windowHeight="15135" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="15960" windowHeight="6510" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Array" sheetId="1" r:id="rId1"/>
     <sheet name="LinkedList" sheetId="2" r:id="rId2"/>
     <sheet name="Stack&amp;Queue" sheetId="3" r:id="rId3"/>
+    <sheet name="HashMap" sheetId="4" r:id="rId4"/>
+    <sheet name="Tree" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:K20"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
   <si>
     <t>Rotate Image</t>
   </si>
@@ -106,6 +109,90 @@
   </si>
   <si>
     <t>Container With Most Water</t>
+  </si>
+  <si>
+    <t>Two Sum</t>
+  </si>
+  <si>
+    <t>Copy List with Random Pointer</t>
+  </si>
+  <si>
+    <t>Valid Sudoku</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Minimum Window Substring </t>
+  </si>
+  <si>
+    <t>Max Points on a Line</t>
+  </si>
+  <si>
+    <t>Longest Substring Without Repeating Characters</t>
+  </si>
+  <si>
+    <t>Anagrams</t>
+  </si>
+  <si>
+    <t>4Sum</t>
+  </si>
+  <si>
+    <t>Binary Tree Preorder Traversal</t>
+  </si>
+  <si>
+    <t>Binary Tree Postorder Traversal</t>
+  </si>
+  <si>
+    <t>Binary Tree Inorder Traversal</t>
+  </si>
+  <si>
+    <t>Binary Tree Level Order Traversal</t>
+  </si>
+  <si>
+    <t>Binary Tree Level Order Traversal II</t>
+  </si>
+  <si>
+    <t>Binary Tree Zigzag Level Order Traversal</t>
+  </si>
+  <si>
+    <t>Construct Binary Tree from Preorder and Inorder Traversal</t>
+  </si>
+  <si>
+    <t>Construct Binary Tree from Inorder and Postorder Traversal</t>
+  </si>
+  <si>
+    <t>Balanced Binary Tree</t>
+  </si>
+  <si>
+    <t>Validate Binary Search Tree</t>
+  </si>
+  <si>
+    <t>Symmetric Tree</t>
+  </si>
+  <si>
+    <t>Same Tree</t>
+  </si>
+  <si>
+    <t>Populating Next Right Pointers in Each Node</t>
+  </si>
+  <si>
+    <t>Populating Next Right Pointers in Each Node II</t>
+  </si>
+  <si>
+    <t>Path Sum</t>
+  </si>
+  <si>
+    <t>Path Sum II</t>
+  </si>
+  <si>
+    <t>Minimum Depth of Binary Tree</t>
+  </si>
+  <si>
+    <t>Maximum Depth of Binary Tree</t>
+  </si>
+  <si>
+    <t>Flatten Binary Tree to Linked List</t>
+  </si>
+  <si>
+    <t>Convert Sorted Array to Binary Search Tree</t>
   </si>
 </sst>
 </file>
@@ -452,7 +539,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38" customWidth="1"/>
+    <col min="1" max="1" width="36.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -524,7 +611,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="45.5703125" customWidth="1"/>
+    <col min="1" max="1" width="34.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -609,13 +696,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38.85546875" customWidth="1"/>
+    <col min="1" max="1" width="31" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -654,4 +741,186 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="44.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A1:A8">
+    <sortCondition ref="A1"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="54.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A1:A20">
+    <sortCondition ref="A1"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
re-org tree folder into 4 seperated folders
</commit_message>
<xml_diff>
--- a/lc/resource/leetcode_category.xlsx
+++ b/lc/resource/leetcode_category.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="15960" windowHeight="6510" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="19245" windowHeight="10470" tabRatio="880" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Array" sheetId="1" r:id="rId1"/>
@@ -12,14 +12,18 @@
     <sheet name="Stack&amp;Queue" sheetId="3" r:id="rId3"/>
     <sheet name="HashMap" sheetId="4" r:id="rId4"/>
     <sheet name="Tree" sheetId="5" r:id="rId5"/>
+    <sheet name="Tree_Traversal" sheetId="7" r:id="rId6"/>
+    <sheet name="Tree_Sum" sheetId="9" r:id="rId7"/>
+    <sheet name="Tree_Nature" sheetId="8" r:id="rId8"/>
+    <sheet name="Tree_Building" sheetId="6" r:id="rId9"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:K20"/>
+  <oleSize ref="A1:Q33"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
   <si>
     <t>Rotate Image</t>
   </si>
@@ -193,6 +197,15 @@
   </si>
   <si>
     <t>Convert Sorted Array to Binary Search Tree</t>
+  </si>
+  <si>
+    <t>Convert Sorted List to Binary Search Tree</t>
+  </si>
+  <si>
+    <t>Sum Root to Leaf Numbers</t>
+  </si>
+  <si>
+    <t>Binary Tree Maximum Path Sum</t>
   </si>
 </sst>
 </file>
@@ -806,10 +819,200 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A20"/>
+  <dimension ref="A1:A21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="42.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="17" spans="1:1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="18" spans="1:1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="1:1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="1:1" customFormat="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <sortState ref="A1:A20">
+    <sortCondition ref="A1"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="36.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A1:A4">
+    <sortCondition ref="A1"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -819,108 +1022,25 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>41</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>47</v>
-      </c>
-    </row>
   </sheetData>
-  <sortState ref="A1:A20">
-    <sortCondition ref="A1"/>
-  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update spreadsheet for question to ask
</commit_message>
<xml_diff>
--- a/lc/resource/leetcode_category.xlsx
+++ b/lc/resource/leetcode_category.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="19245" windowHeight="10470" tabRatio="880" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="16365" windowHeight="6630" tabRatio="880" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Array" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Tree_Building" sheetId="6" r:id="rId9"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:Q33"/>
+  <oleSize ref="A1:M20"/>
 </workbook>
 </file>
 
@@ -821,7 +821,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
@@ -927,7 +927,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
update question to ask
</commit_message>
<xml_diff>
--- a/lc/resource/leetcode_category.xlsx
+++ b/lc/resource/leetcode_category.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="16365" windowHeight="6630" tabRatio="880" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="16365" windowHeight="6630" tabRatio="880" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Array" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
   <si>
     <t>Rotate Image</t>
   </si>
@@ -206,6 +206,15 @@
   </si>
   <si>
     <t>Binary Tree Maximum Path Sum</t>
+  </si>
+  <si>
+    <t>//为什么要先把root加进去？为什么上面的只一行的方法不行？</t>
+  </si>
+  <si>
+    <t>算法的本质是一次先序遍历（为啥？）</t>
+  </si>
+  <si>
+    <t>//item.clear();【注】，这样写错误！原因问问老师。</t>
   </si>
 </sst>
 </file>
@@ -241,8 +250,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -821,7 +831,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
@@ -877,10 +887,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -888,32 +898,35 @@
     <col min="1" max="1" width="36.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>43</v>
       </c>
@@ -925,10 +938,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -936,24 +949,30 @@
     <col min="1" max="1" width="29.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>59</v>
+      </c>
+      <c r="B4" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
rename source folder Tree_Building into Tree_Construct
</commit_message>
<xml_diff>
--- a/lc/resource/leetcode_category.xlsx
+++ b/lc/resource/leetcode_category.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="16365" windowHeight="6630" tabRatio="880" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="16365" windowHeight="6630" tabRatio="880" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Array" sheetId="1" r:id="rId1"/>
@@ -15,10 +15,10 @@
     <sheet name="Tree_Traversal" sheetId="7" r:id="rId6"/>
     <sheet name="Tree_Sum" sheetId="9" r:id="rId7"/>
     <sheet name="Tree_Nature" sheetId="8" r:id="rId8"/>
-    <sheet name="Tree_Building" sheetId="6" r:id="rId9"/>
+    <sheet name="Tree_Construct" sheetId="6" r:id="rId9"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:M20"/>
+  <oleSize ref="A1:K20"/>
 </workbook>
 </file>
 
@@ -889,7 +889,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -1030,8 +1030,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
add category for Binary_Search
</commit_message>
<xml_diff>
--- a/lc/resource/leetcode_category.xlsx
+++ b/lc/resource/leetcode_category.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="16365" windowHeight="6630" tabRatio="880" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="19725" windowHeight="10470" tabRatio="880" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Array" sheetId="1" r:id="rId1"/>
@@ -16,14 +16,15 @@
     <sheet name="Tree_Sum" sheetId="9" r:id="rId7"/>
     <sheet name="Tree_Nature" sheetId="8" r:id="rId8"/>
     <sheet name="Tree_Construct" sheetId="6" r:id="rId9"/>
+    <sheet name="Binary_Search" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:K20"/>
+  <oleSize ref="A1:T33"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
   <si>
     <t>Rotate Image</t>
   </si>
@@ -215,6 +216,24 @@
   </si>
   <si>
     <t>//item.clear();【注】，这样写错误！原因问问老师。</t>
+  </si>
+  <si>
+    <t>Search Insert Position</t>
+  </si>
+  <si>
+    <t>Search for a Range</t>
+  </si>
+  <si>
+    <t>Sqrt(x)</t>
+  </si>
+  <si>
+    <t>Search a 2D Matrix</t>
+  </si>
+  <si>
+    <t>Search in Rotated Sorted Array</t>
+  </si>
+  <si>
+    <t>Search in Rotated Sorted Array II</t>
   </si>
 </sst>
 </file>
@@ -624,6 +643,57 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A1:A6">
+    <sortCondition ref="A1"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A14"/>
@@ -1030,7 +1100,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Adding Sort and Divide&Conquer category and regroup some other categories
</commit_message>
<xml_diff>
--- a/lc/resource/leetcode_category.xlsx
+++ b/lc/resource/leetcode_category.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="14025" windowHeight="5670" tabRatio="880" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="14145" windowHeight="6165" tabRatio="880" firstSheet="4" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Array" sheetId="1" r:id="rId1"/>
@@ -17,14 +17,16 @@
     <sheet name="Tree_Nature" sheetId="8" r:id="rId8"/>
     <sheet name="Tree_Construct" sheetId="6" r:id="rId9"/>
     <sheet name="Binary_Search" sheetId="10" r:id="rId10"/>
+    <sheet name="Sort" sheetId="11" r:id="rId11"/>
+    <sheet name="Divide&amp;Conquer" sheetId="12" r:id="rId12"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:I17"/>
+  <oleSize ref="A1:J19"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="94">
   <si>
     <t>Rotate Image</t>
   </si>
@@ -237,6 +239,75 @@
   </si>
   <si>
     <t>//helper里，左根右，关于根的处理，没看懂</t>
+  </si>
+  <si>
+    <t>Sort List</t>
+  </si>
+  <si>
+    <t>Insertion Sort List</t>
+  </si>
+  <si>
+    <t>Insert Interval</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Merge Intervals </t>
+  </si>
+  <si>
+    <t>(第一周留过)</t>
+  </si>
+  <si>
+    <t>Median of Two Sorted Arrays</t>
+  </si>
+  <si>
+    <t>Find Minimum in Rotated Sorted Array</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Find Minimum in Rotated Sorted Array II </t>
+  </si>
+  <si>
+    <t>Pow(x, n)</t>
+  </si>
+  <si>
+    <t>Divide Two Integers</t>
+  </si>
+  <si>
+    <t>Single Number</t>
+  </si>
+  <si>
+    <t>Add Binary</t>
+  </si>
+  <si>
+    <t>Implement strStr()</t>
+  </si>
+  <si>
+    <t>Min Stack</t>
+  </si>
+  <si>
+    <t>LRU Cache</t>
+  </si>
+  <si>
+    <t>3 Sum</t>
+  </si>
+  <si>
+    <t>3 Sum Closest</t>
+  </si>
+  <si>
+    <t>Spiral Matrix</t>
+  </si>
+  <si>
+    <t>Spiral Matrix II</t>
+  </si>
+  <si>
+    <t>LinkedList</t>
+  </si>
+  <si>
+    <t>Array</t>
+  </si>
+  <si>
+    <t>Tree_Construct</t>
+  </si>
+  <si>
+    <t>Two_Pointers</t>
   </si>
 </sst>
 </file>
@@ -252,12 +323,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -272,9 +349,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -648,49 +727,224 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37.42578125" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2" s="2"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B3" s="2"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B4" s="2"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B6" s="2"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25"/>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <sortState ref="A1:A18">
+    <sortCondition ref="A1"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+      <c r="C5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A1:B5">
+    <sortCondition ref="A1"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>66</v>
+        <v>84</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>89</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A1:A6">
+  <sortState ref="A1:A9">
     <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1103,7 +1357,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
add DP_1D and DP_2D categories
</commit_message>
<xml_diff>
--- a/lc/resource/leetcode_category.xlsx
+++ b/lc/resource/leetcode_category.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="14145" windowHeight="6165" tabRatio="880" firstSheet="4" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="14145" windowHeight="6165" tabRatio="880" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="Array" sheetId="1" r:id="rId1"/>
@@ -19,14 +19,15 @@
     <sheet name="Binary_Search" sheetId="10" r:id="rId10"/>
     <sheet name="Sort" sheetId="11" r:id="rId11"/>
     <sheet name="Divide&amp;Conquer" sheetId="12" r:id="rId12"/>
+    <sheet name="DP_1D" sheetId="13" r:id="rId13"/>
+    <sheet name="DP_2D" sheetId="14" r:id="rId14"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:J19"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="110">
   <si>
     <t>Rotate Image</t>
   </si>
@@ -308,6 +309,54 @@
   </si>
   <si>
     <t>Two_Pointers</t>
+  </si>
+  <si>
+    <t>用mo的方法试试</t>
+  </si>
+  <si>
+    <t>改成BFS模板</t>
+  </si>
+  <si>
+    <t>Climbing Stairs</t>
+  </si>
+  <si>
+    <t>Decode Ways</t>
+  </si>
+  <si>
+    <t>Unique Binary Search Trees</t>
+  </si>
+  <si>
+    <t>Maximum Subarray</t>
+  </si>
+  <si>
+    <t>Maximum Product Subarray</t>
+  </si>
+  <si>
+    <t>Best Time to Buy and Sell Stock</t>
+  </si>
+  <si>
+    <t>Jump Game</t>
+  </si>
+  <si>
+    <t>Jump Game II</t>
+  </si>
+  <si>
+    <t>Palindrome Partitioning</t>
+  </si>
+  <si>
+    <t>Palindrome Partitioning II</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Longest Consecutive Sequence </t>
+  </si>
+  <si>
+    <t>Edit Distance</t>
+  </si>
+  <si>
+    <t>Distinct Subsequences</t>
+  </si>
+  <si>
+    <t>Interleaving String</t>
   </si>
 </sst>
 </file>
@@ -727,10 +776,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -752,19 +801,19 @@
       <c r="A2" t="s">
         <v>80</v>
       </c>
-      <c r="B2" s="2"/>
+      <c r="B2" s="3"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>77</v>
       </c>
-      <c r="B3" s="2"/>
+      <c r="B3" s="3"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>78</v>
       </c>
-      <c r="B4" s="2"/>
+      <c r="B4" s="3"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -807,12 +856,6 @@
         <v>66</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25"/>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <sortState ref="A1:A18">
     <sortCondition ref="A1"/>
@@ -826,7 +869,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -840,22 +883,25 @@
       <c r="A1" t="s">
         <v>73</v>
       </c>
+      <c r="B1" s="2"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>72</v>
       </c>
+      <c r="B2" s="2"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>74</v>
       </c>
+      <c r="B3" s="2"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="3" t="s">
         <v>75</v>
       </c>
       <c r="C4" t="s">
@@ -866,6 +912,7 @@
       <c r="A5" t="s">
         <v>71</v>
       </c>
+      <c r="B5" s="3"/>
       <c r="C5" t="s">
         <v>90</v>
       </c>
@@ -883,7 +930,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -912,39 +959,158 @@
       <c r="A3" t="s">
         <v>82</v>
       </c>
+      <c r="B3" s="2"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>83</v>
       </c>
+      <c r="B4" s="2"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>85</v>
       </c>
+      <c r="B5" s="2"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>84</v>
       </c>
+      <c r="B6" s="2"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>81</v>
       </c>
+      <c r="B7" s="2"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>88</v>
       </c>
+      <c r="B8" s="2"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>89</v>
       </c>
+      <c r="B9" s="2"/>
     </row>
   </sheetData>
   <sortState ref="A1:A9">
+    <sortCondition ref="A1"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>98</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A1:A6">
+    <sortCondition ref="A1"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>105</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A1:A8">
     <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1044,10 +1210,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1055,32 +1221,33 @@
     <col min="1" max="1" width="31" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B3" s="2"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -1095,7 +1262,69 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A8"/>
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="44.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="2"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A1:A8">
+    <sortCondition ref="A1"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
@@ -1103,107 +1332,31 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="44.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-  </sheetData>
-  <sortState ref="A1:A8">
-    <sortCondition ref="A1"/>
-  </sortState>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A21"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
     <col min="1" max="1" width="42.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="2"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="2"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="17" spans="1:1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="18" spans="1:1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="19" spans="1:1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="20" spans="1:1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="21" spans="1:1" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <sortState ref="A1:A20">
     <sortCondition ref="A1"/>
@@ -1214,23 +1367,29 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="36.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B1" s="2"/>
+      <c r="C1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>41</v>
       </c>
@@ -1238,22 +1397,31 @@
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B3" s="2"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B4" s="2"/>
+      <c r="C4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B5" s="2"/>
+      <c r="C5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>43</v>
       </c>
@@ -1268,12 +1436,13 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="61.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -1290,7 +1459,7 @@
       <c r="A3" t="s">
         <v>53</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1298,7 +1467,7 @@
       <c r="A4" t="s">
         <v>59</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>62</v>
       </c>
     </row>
@@ -1312,38 +1481,47 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B2" s="2"/>
+      <c r="C2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B3" s="2"/>
+      <c r="C3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>48</v>
       </c>
@@ -1358,7 +1536,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1379,18 +1557,21 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B3" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>57</v>
+        <v>58</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A1:B4">
+    <sortCondition ref="A1"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
group DP_1D and DP_2D
</commit_message>
<xml_diff>
--- a/lc/resource/leetcode_category.xlsx
+++ b/lc/resource/leetcode_category.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="14145" windowHeight="6165" tabRatio="880" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="14145" windowHeight="6165" tabRatio="880" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="Array" sheetId="1" r:id="rId1"/>
@@ -1004,10 +1004,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1015,35 +1015,41 @@
     <col min="1" max="1" width="28.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B1" s="2"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B2" s="2"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B3" s="2"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B4" s="2"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B5" s="2"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>97</v>
       </c>
+      <c r="B6" s="2"/>
     </row>
   </sheetData>
   <sortState ref="A1:A6">
@@ -1055,10 +1061,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A8"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1066,45 +1072,53 @@
     <col min="1" max="1" width="29.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B1" s="2"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B2" s="2"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B3" s="2"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B4" s="2"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B5" s="2"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B6" s="2"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B7" s="2"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>104</v>
       </c>
+      <c r="B8" s="2"/>
     </row>
   </sheetData>
   <sortState ref="A1:A8">
@@ -1323,7 +1337,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
re-group DP into 4 sub groups
</commit_message>
<xml_diff>
--- a/lc/resource/leetcode_category.xlsx
+++ b/lc/resource/leetcode_category.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="14145" windowHeight="6165" tabRatio="880" activeTab="12"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="14145" windowHeight="6165" tabRatio="880" firstSheet="9" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="Array" sheetId="1" r:id="rId1"/>
@@ -19,15 +19,17 @@
     <sheet name="Binary_Search" sheetId="10" r:id="rId10"/>
     <sheet name="Sort" sheetId="11" r:id="rId11"/>
     <sheet name="Divide&amp;Conquer" sheetId="12" r:id="rId12"/>
-    <sheet name="DP_1D" sheetId="13" r:id="rId13"/>
-    <sheet name="DP_2D" sheetId="14" r:id="rId14"/>
+    <sheet name="DP_Matrix" sheetId="13" r:id="rId13"/>
+    <sheet name="DP_Sequence" sheetId="14" r:id="rId14"/>
+    <sheet name="DP_2_Sequence" sheetId="15" r:id="rId15"/>
+    <sheet name="DP_Backpack" sheetId="16" r:id="rId16"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="112">
   <si>
     <t>Rotate Image</t>
   </si>
@@ -338,9 +340,6 @@
     <t>Jump Game II</t>
   </si>
   <si>
-    <t>Palindrome Partitioning</t>
-  </si>
-  <si>
     <t>Palindrome Partitioning II</t>
   </si>
   <si>
@@ -354,16 +353,35 @@
   </si>
   <si>
     <t>Interleaving String</t>
+  </si>
+  <si>
+    <t>Tiangle</t>
+  </si>
+  <si>
+    <t>Unique Paths</t>
+  </si>
+  <si>
+    <t>Unique Paths II</t>
+  </si>
+  <si>
+    <t>Minimum Path Sum</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -395,11 +413,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1004,10 +1023,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B6"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1023,25 +1042,25 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="B2" s="2"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B3" s="2"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>99</v>
+        <v>111</v>
       </c>
       <c r="B4" s="2"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="B5" s="2"/>
     </row>
@@ -1051,8 +1070,20 @@
       </c>
       <c r="B6" s="2"/>
     </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>109</v>
+      </c>
+      <c r="B7" s="2"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>110</v>
+      </c>
+      <c r="B8" s="2"/>
+    </row>
   </sheetData>
-  <sortState ref="A1:A6">
+  <sortState ref="A1:A8">
     <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1061,10 +1092,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1074,56 +1105,102 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>107</v>
-      </c>
-      <c r="B1" s="2"/>
+        <v>95</v>
+      </c>
+      <c r="B1" s="4"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>106</v>
-      </c>
-      <c r="B2" s="2"/>
+        <v>96</v>
+      </c>
+      <c r="B2" s="4"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="B3" s="2"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B4" s="2"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B5" s="2"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B6" s="2"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>103</v>
-      </c>
-      <c r="B7" s="2"/>
+      <c r="B7" s="3"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>104</v>
-      </c>
-      <c r="B8" s="2"/>
+      <c r="B8" s="3"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B9" s="3"/>
     </row>
   </sheetData>
-  <sortState ref="A1:A8">
+  <sortState ref="A1:A13">
     <sortCondition ref="A1"/>
   </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B1" s="2"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B2" s="2"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B3" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
update spreadsheet and upload leetcodeBlog
</commit_message>
<xml_diff>
--- a/lc/resource/leetcode_category.xlsx
+++ b/lc/resource/leetcode_category.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="14145" windowHeight="6165" tabRatio="880" firstSheet="9" activeTab="12"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="14145" windowHeight="6165" tabRatio="880" firstSheet="2" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="Array" sheetId="1" r:id="rId1"/>
@@ -24,12 +24,12 @@
     <sheet name="DP_2_Sequence" sheetId="15" r:id="rId15"/>
     <sheet name="DP_Backpack" sheetId="16" r:id="rId16"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="111">
   <si>
     <t>Rotate Image</t>
   </si>
@@ -214,12 +214,6 @@
     <t>Binary Tree Maximum Path Sum</t>
   </si>
   <si>
-    <t>//为什么要先把root加进去？为什么上面的只一行的方法不行？</t>
-  </si>
-  <si>
-    <t>算法的本质是一次先序遍历（为啥？）</t>
-  </si>
-  <si>
     <t>//item.clear();【注】，这样写错误！原因问问老师。</t>
   </si>
   <si>
@@ -313,9 +307,6 @@
     <t>Two_Pointers</t>
   </si>
   <si>
-    <t>用mo的方法试试</t>
-  </si>
-  <si>
     <t>Climbing Stairs</t>
   </si>
   <si>
@@ -355,9 +346,6 @@
     <t>Interleaving String</t>
   </si>
   <si>
-    <t>Tiangle</t>
-  </si>
-  <si>
     <t>Unique Paths</t>
   </si>
   <si>
@@ -365,6 +353,15 @@
   </si>
   <si>
     <t>Minimum Path Sum</t>
+  </si>
+  <si>
+    <t>//操作完叶子节点之后为什么要solution.remove(solution.size()-1);</t>
+  </si>
+  <si>
+    <t>Triangle</t>
+  </si>
+  <si>
+    <t>//【注】，为什么在这里就可以跳出了？而不需要列出所有可行的j，然后再找其中的最小值？</t>
   </si>
 </sst>
 </file>
@@ -795,7 +792,7 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -810,66 +807,66 @@
       </c>
       <c r="B1" s="3"/>
       <c r="C1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B2" s="3"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B3" s="3"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B4" s="3"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B6" s="2"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -885,7 +882,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -897,40 +894,40 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>73</v>
-      </c>
-      <c r="B1" s="2"/>
+        <v>71</v>
+      </c>
+      <c r="B1" s="3"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B2" s="2"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>74</v>
-      </c>
-      <c r="B3" s="2"/>
+        <v>72</v>
+      </c>
+      <c r="B3" s="3"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -957,59 +954,59 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B3" s="2"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B4" s="2"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B5" s="2"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B6" s="2"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B7" s="2"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B8" s="2"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B9" s="2"/>
     </row>
@@ -1023,10 +1020,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1036,54 +1033,58 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B1" s="2"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>99</v>
-      </c>
-      <c r="B2" s="2"/>
+        <v>92</v>
+      </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B3" s="2"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>111</v>
+        <v>95</v>
       </c>
       <c r="B4" s="2"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>108</v>
-      </c>
-      <c r="B5" s="2"/>
+        <v>107</v>
+      </c>
+      <c r="B5" s="3"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>97</v>
+        <v>109</v>
       </c>
       <c r="B6" s="2"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>109</v>
-      </c>
-      <c r="B7" s="2"/>
+        <v>94</v>
+      </c>
+      <c r="B7" s="3"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>110</v>
-      </c>
-      <c r="B8" s="2"/>
+        <v>105</v>
+      </c>
+      <c r="B8" s="3"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>106</v>
+      </c>
     </row>
   </sheetData>
-  <sortState ref="A1:A8">
+  <sortState ref="A1:A9">
     <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1092,68 +1093,65 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="91.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B1" s="4"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>96</v>
-      </c>
-      <c r="B2" s="4"/>
+        <v>98</v>
+      </c>
+      <c r="B2" s="3"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>101</v>
-      </c>
-      <c r="B3" s="2"/>
+        <v>99</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B4" s="2"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B5" s="2"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>103</v>
-      </c>
-      <c r="B6" s="2"/>
+      <c r="B6" s="3"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" s="3"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B8" s="3"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B9" s="3"/>
     </row>
   </sheetData>
   <sortState ref="A1:A13">
     <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1172,19 +1170,19 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B1" s="2"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B2" s="2"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B3" s="2"/>
     </row>
@@ -1415,7 +1413,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1432,13 +1430,13 @@
       <c r="A2" t="s">
         <v>50</v>
       </c>
-      <c r="B2" s="2"/>
+      <c r="B2" s="3"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>51</v>
       </c>
-      <c r="B3" s="2"/>
+      <c r="B3" s="3"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -1455,10 +1453,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C1" sqref="C1:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1468,48 +1466,39 @@
     <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B1" s="3"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>41</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>42</v>
       </c>
       <c r="B3" s="3"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>39</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B4" s="3"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>38</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B5" s="3"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>43</v>
       </c>
@@ -1524,7 +1513,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1548,16 +1537,14 @@
         <v>53</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>61</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>59</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>62</v>
-      </c>
+      <c r="B4" s="3"/>
     </row>
   </sheetData>
   <sortState ref="A1:A4">
@@ -1618,7 +1605,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1647,7 +1634,7 @@
         <v>58</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1655,5 +1642,6 @@
     <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
regroup and refactor LRU_Cache
</commit_message>
<xml_diff>
--- a/lc/resource/leetcode_category.xlsx
+++ b/lc/resource/leetcode_category.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="14145" windowHeight="6165" tabRatio="880" firstSheet="13" activeTab="16"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="14145" windowHeight="6165" tabRatio="880" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Array" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="125">
   <si>
     <t>Rotate Image</t>
   </si>
@@ -402,6 +402,9 @@
   </si>
   <si>
     <t>Word_Ladder II</t>
+  </si>
+  <si>
+    <t>Longest Consecutive Sequence</t>
   </si>
 </sst>
 </file>
@@ -980,10 +983,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1022,33 +1025,27 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B5" s="2"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B6" s="2"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="B7" s="2"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B8" s="2"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>87</v>
-      </c>
-      <c r="B9" s="2"/>
     </row>
   </sheetData>
   <sortState ref="A1:A9">
@@ -1063,7 +1060,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1253,7 +1250,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
@@ -1484,10 +1481,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1497,50 +1494,62 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B1" s="2"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>34</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>30</v>
+        <v>124</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>32</v>
-      </c>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" s="2"/>
     </row>
   </sheetData>
-  <sortState ref="A1:A8">
-    <sortCondition ref="A1"/>
+  <sortState ref="A1:A10">
+    <sortCondition descending="1" ref="A1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
update and regroup Maximum_Subarray
</commit_message>
<xml_diff>
--- a/lc/resource/leetcode_category.xlsx
+++ b/lc/resource/leetcode_category.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="14145" windowHeight="6165" tabRatio="880" activeTab="11"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="14145" windowHeight="6165" tabRatio="880" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="Array" sheetId="1" r:id="rId1"/>
@@ -985,7 +985,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
@@ -1057,10 +1057,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1087,36 +1087,30 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>95</v>
-      </c>
-      <c r="B4" s="2"/>
+        <v>107</v>
+      </c>
+      <c r="B4" s="3"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>107</v>
-      </c>
-      <c r="B5" s="3"/>
+        <v>109</v>
+      </c>
+      <c r="B5" s="2"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>109</v>
+        <v>94</v>
       </c>
       <c r="B6" s="2"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>94</v>
-      </c>
-      <c r="B7" s="2"/>
+        <v>105</v>
+      </c>
+      <c r="B7" s="3"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>105</v>
-      </c>
-      <c r="B8" s="3"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
         <v>106</v>
       </c>
     </row>
@@ -1133,7 +1127,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="F47" sqref="F47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1175,6 +1169,9 @@
       <c r="B5" s="3"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>95</v>
+      </c>
       <c r="B6" s="3"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
update and regroup Unique_Binary_Search_Trees
</commit_message>
<xml_diff>
--- a/lc/resource/leetcode_category.xlsx
+++ b/lc/resource/leetcode_category.xlsx
@@ -1054,10 +1054,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1090,18 +1090,12 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>94</v>
-      </c>
-      <c r="B5" s="2"/>
+        <v>104</v>
+      </c>
+      <c r="B5" s="3"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>104</v>
-      </c>
-      <c r="B6" s="3"/>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
         <v>105</v>
       </c>
     </row>
@@ -1110,6 +1104,7 @@
     <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1118,7 +1113,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1166,7 +1161,10 @@
       <c r="B6" s="3"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B7" s="3"/>
+      <c r="A7" t="s">
+        <v>94</v>
+      </c>
+      <c r="B7" s="2"/>
     </row>
   </sheetData>
   <sortState ref="A1:B8">

</xml_diff>

<commit_message>
update and regroup Gray_Code
</commit_message>
<xml_diff>
--- a/lc/resource/leetcode_category.xlsx
+++ b/lc/resource/leetcode_category.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="14145" windowHeight="6165" tabRatio="899" firstSheet="2" activeTab="16"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="14145" windowHeight="6165" tabRatio="899" firstSheet="2" activeTab="18"/>
   </bookViews>
   <sheets>
     <sheet name="Array" sheetId="1" r:id="rId1"/>
@@ -1140,7 +1140,7 @@
     <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1277,8 +1277,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A15" sqref="A15:B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1308,7 +1308,7 @@
       <c r="A4" t="s">
         <v>126</v>
       </c>
-      <c r="B4" s="2"/>
+      <c r="B4" s="3"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -1355,7 +1355,7 @@
       <c r="A12" t="s">
         <v>125</v>
       </c>
-      <c r="B12" s="2"/>
+      <c r="B12" s="3"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -1366,12 +1366,6 @@
       <c r="A14" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>127</v>
-      </c>
-      <c r="B15" s="2"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -1426,10 +1420,10 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1437,10 +1431,17 @@
     <col min="1" max="1" width="21.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>124</v>
       </c>
+      <c r="B1" s="2"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B2" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1660,7 +1661,7 @@
     <sortCondition descending="1" ref="A1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
update spreadsheet for categorizing questions
</commit_message>
<xml_diff>
--- a/lc/resource/leetcode_category.xlsx
+++ b/lc/resource/leetcode_category.xlsx
@@ -4,35 +4,43 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="14145" windowHeight="6165" tabRatio="899" firstSheet="2" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="14145" windowHeight="6165" tabRatio="899"/>
   </bookViews>
   <sheets>
-    <sheet name="Array" sheetId="1" r:id="rId1"/>
-    <sheet name="LinkedList" sheetId="2" r:id="rId2"/>
-    <sheet name="Stack&amp;Queue" sheetId="3" r:id="rId3"/>
-    <sheet name="HashMap" sheetId="4" r:id="rId4"/>
-    <sheet name="Tree" sheetId="5" r:id="rId5"/>
-    <sheet name="Tree_Traversal" sheetId="7" r:id="rId6"/>
-    <sheet name="Tree_Sum" sheetId="9" r:id="rId7"/>
-    <sheet name="Tree_Nature" sheetId="8" r:id="rId8"/>
-    <sheet name="Tree_Construct" sheetId="6" r:id="rId9"/>
-    <sheet name="Binary_Search" sheetId="10" r:id="rId10"/>
-    <sheet name="Sort" sheetId="11" r:id="rId11"/>
-    <sheet name="Divide&amp;Conquer" sheetId="12" r:id="rId12"/>
-    <sheet name="DP_Matrix" sheetId="13" r:id="rId13"/>
-    <sheet name="DP_1_Sequence" sheetId="14" r:id="rId14"/>
-    <sheet name="DP_2_Sequence" sheetId="15" r:id="rId15"/>
-    <sheet name="DP_Backpack" sheetId="16" r:id="rId16"/>
-    <sheet name="Graph&amp;Search" sheetId="17" r:id="rId17"/>
-    <sheet name="High_Frequency" sheetId="18" r:id="rId18"/>
-    <sheet name="Math" sheetId="19" r:id="rId19"/>
+    <sheet name="Matrix" sheetId="20" r:id="rId1"/>
+    <sheet name="Array" sheetId="1" r:id="rId2"/>
+    <sheet name="LinkedList" sheetId="2" r:id="rId3"/>
+    <sheet name="Stack&amp;Queue" sheetId="3" r:id="rId4"/>
+    <sheet name="HashMap" sheetId="4" r:id="rId5"/>
+    <sheet name="Tree" sheetId="5" r:id="rId6"/>
+    <sheet name="Tree_Traversal" sheetId="7" r:id="rId7"/>
+    <sheet name="Tree_Sum" sheetId="9" r:id="rId8"/>
+    <sheet name="Tree_Nature" sheetId="8" r:id="rId9"/>
+    <sheet name="Tree_Construct" sheetId="6" r:id="rId10"/>
+    <sheet name="Binary_Search" sheetId="10" r:id="rId11"/>
+    <sheet name="Sort" sheetId="11" r:id="rId12"/>
+    <sheet name="Divide&amp;Conquer" sheetId="12" r:id="rId13"/>
+    <sheet name="DP_Matrix" sheetId="13" r:id="rId14"/>
+    <sheet name="DP_1_Sequence" sheetId="14" r:id="rId15"/>
+    <sheet name="DP_2_Sequence" sheetId="15" r:id="rId16"/>
+    <sheet name="DP_Backpack" sheetId="16" r:id="rId17"/>
+    <sheet name="Graph&amp;Search" sheetId="17" r:id="rId18"/>
+    <sheet name="High_Frequency" sheetId="18" r:id="rId19"/>
+    <sheet name="Math" sheetId="19" r:id="rId20"/>
+    <sheet name="High_Accuracy" sheetId="21" r:id="rId21"/>
+    <sheet name="String" sheetId="22" r:id="rId22"/>
+    <sheet name="Two_Pointers" sheetId="23" r:id="rId23"/>
+    <sheet name="Sheet5" sheetId="24" r:id="rId24"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Matrix!$A$1:$G$159</definedName>
+  </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="974" uniqueCount="208">
   <si>
     <t>Rotate Image</t>
   </si>
@@ -253,9 +261,6 @@
     <t xml:space="preserve">Merge Intervals </t>
   </si>
   <si>
-    <t>(第一周留过)</t>
-  </si>
-  <si>
     <t>Median of Two Sorted Arrays</t>
   </si>
   <si>
@@ -355,9 +360,6 @@
     <t>Minimum Path Sum</t>
   </si>
   <si>
-    <t>//操作完叶子节点之后为什么要solution.remove(solution.size()-1);</t>
-  </si>
-  <si>
     <t>Triangle</t>
   </si>
   <si>
@@ -394,12 +396,6 @@
     <t>Subsets II</t>
   </si>
   <si>
-    <t>Word_Ladder</t>
-  </si>
-  <si>
-    <t>Word_Ladder II</t>
-  </si>
-  <si>
     <t>Longest Consecutive Sequence</t>
   </si>
   <si>
@@ -433,7 +429,241 @@
     <t>Sudoku Solver</t>
   </si>
   <si>
-    <t>Implement Queue by  Stacks</t>
+    <t>Best Time to Buy and Sell Stock II</t>
+  </si>
+  <si>
+    <t>Best Time to Buy and Sell Stock III</t>
+  </si>
+  <si>
+    <t>Question Name</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Question Source</t>
+  </si>
+  <si>
+    <t>Question Link</t>
+  </si>
+  <si>
+    <t>Solution Link</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>Set_Matrix_Zeroes</t>
+  </si>
+  <si>
+    <t>Spiral_Matrix</t>
+  </si>
+  <si>
+    <t>Spiral_Matrix_II</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>leetcode</t>
+  </si>
+  <si>
+    <t>Set Matrix Zeroes</t>
+  </si>
+  <si>
+    <t>Binary_Search</t>
+  </si>
+  <si>
+    <t>Candy</t>
+  </si>
+  <si>
+    <t>Longest Palindromic Substring</t>
+  </si>
+  <si>
+    <t>Word Break</t>
+  </si>
+  <si>
+    <t>DP_1_Sequence</t>
+  </si>
+  <si>
+    <t>Scramble String</t>
+  </si>
+  <si>
+    <t>DP_2_Sequence</t>
+  </si>
+  <si>
+    <t>DP_Matrix</t>
+  </si>
+  <si>
+    <t>Combinations</t>
+  </si>
+  <si>
+    <t>Word Ladder</t>
+  </si>
+  <si>
+    <t>Word Ladder II</t>
+  </si>
+  <si>
+    <t>Surrounded Regions</t>
+  </si>
+  <si>
+    <t>Graph&amp;Search</t>
+  </si>
+  <si>
+    <t>Substring_with_Concatenation_of_All_Words</t>
+  </si>
+  <si>
+    <t>HashMap</t>
+  </si>
+  <si>
+    <t>Multiply Strings</t>
+  </si>
+  <si>
+    <t>String to Integer_atoi</t>
+  </si>
+  <si>
+    <t>Valid Number</t>
+  </si>
+  <si>
+    <t>Gas Station</t>
+  </si>
+  <si>
+    <t>Majority Element</t>
+  </si>
+  <si>
+    <t>Next Permutation</t>
+  </si>
+  <si>
+    <t>Palindrome Number</t>
+  </si>
+  <si>
+    <t>Reverse Integer</t>
+  </si>
+  <si>
+    <t>Single Number_II</t>
+  </si>
+  <si>
+    <t>Math</t>
+  </si>
+  <si>
+    <t>N_Sum</t>
+  </si>
+  <si>
+    <t>3Sum</t>
+  </si>
+  <si>
+    <t>3Sum_Closest</t>
+  </si>
+  <si>
+    <t>Two Sum III - Data structure design</t>
+  </si>
+  <si>
+    <t>Two Sum II - Input array is sorted</t>
+  </si>
+  <si>
+    <t>Sort</t>
+  </si>
+  <si>
+    <t>Longest Valid Parentheses</t>
+  </si>
+  <si>
+    <t>Maximal_ Rectangle</t>
+  </si>
+  <si>
+    <t>Stack&amp;Queue</t>
+  </si>
+  <si>
+    <t>Reverse_Words_in_a_String</t>
+  </si>
+  <si>
+    <t>Count and Say</t>
+  </si>
+  <si>
+    <t>Integer to Roman</t>
+  </si>
+  <si>
+    <t>Length of Last Word</t>
+  </si>
+  <si>
+    <t>Longest Common Prefix</t>
+  </si>
+  <si>
+    <t>Roman to Integer</t>
+  </si>
+  <si>
+    <t>Text Justification</t>
+  </si>
+  <si>
+    <t>ZigZag Conversion</t>
+  </si>
+  <si>
+    <t>String</t>
+  </si>
+  <si>
+    <t>This group need to be further split into specific groups</t>
+  </si>
+  <si>
+    <t>Tree</t>
+  </si>
+  <si>
+    <t>Tree_Nature</t>
+  </si>
+  <si>
+    <t>Tree_Sum</t>
+  </si>
+  <si>
+    <t>Tree_Traversal</t>
+  </si>
+  <si>
+    <t>Implement_strStr</t>
+  </si>
+  <si>
+    <t>Valid_Palindrome</t>
+  </si>
+  <si>
+    <t>Implement strStr</t>
+  </si>
+  <si>
+    <t>String to Integer (atoi)</t>
+  </si>
+  <si>
+    <t>3Sum Closest</t>
+  </si>
+  <si>
+    <t>Substring with Concatenation of All Words</t>
+  </si>
+  <si>
+    <t>N-Queens</t>
+  </si>
+  <si>
+    <t>N-Queens II</t>
+  </si>
+  <si>
+    <t>Merge Intervals</t>
+  </si>
+  <si>
+    <t>Minimum Window Substring</t>
+  </si>
+  <si>
+    <t>Maximal Rectangle</t>
+  </si>
+  <si>
+    <t>Recover Binary Search Tree</t>
+  </si>
+  <si>
+    <t>Valid Palindrome</t>
+  </si>
+  <si>
+    <t>Single Number II</t>
+  </si>
+  <si>
+    <t>Reverse Words in a String</t>
+  </si>
+  <si>
+    <t>Find Minimum in Rotated Sorted Array II</t>
+  </si>
+  <si>
+    <t>High_Accuracy</t>
   </si>
 </sst>
 </file>
@@ -462,7 +692,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -475,8 +705,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -484,17 +720,41 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -796,69 +1056,1868 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A10"/>
+  <dimension ref="A1:G159"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="54.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="50" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="D2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="D3" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="D4" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="D5" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="D6" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="D7" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="D8" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="D9" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="D10" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>137</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="D11" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>138</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="D12" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>139</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="D13" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>77</v>
+      </c>
+      <c r="B14" s="3"/>
+      <c r="C14" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="D14" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>74</v>
+      </c>
+      <c r="B15" s="3"/>
+      <c r="C15" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="D15" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>75</v>
+      </c>
+      <c r="B16" s="3"/>
+      <c r="C16" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="D16" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>73</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="D17" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>76</v>
+      </c>
+      <c r="B18" s="2"/>
+      <c r="C18" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="D18" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>65</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="D19" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>63</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="D20" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>66</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="D21" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>67</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="D22" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>62</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="D23" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>64</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="D24" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>96</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="D25" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>130</v>
+      </c>
+      <c r="B26" s="2"/>
+      <c r="C26" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="D26" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>144</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="D27" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>92</v>
+      </c>
+      <c r="B28" s="4"/>
+      <c r="C28" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="D28" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>97</v>
+      </c>
+      <c r="B29" s="3"/>
+      <c r="C29" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="D29" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>98</v>
+      </c>
+      <c r="B30" s="3"/>
+      <c r="C30" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="D30" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>145</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="D31" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>95</v>
+      </c>
+      <c r="B32" s="3"/>
+      <c r="C32" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="D32" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>94</v>
+      </c>
+      <c r="B33" s="3"/>
+      <c r="C33" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="D33" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>99</v>
+      </c>
+      <c r="B34" s="3"/>
+      <c r="C34" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="D34" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>28</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="D35" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>93</v>
+      </c>
+      <c r="B36" s="3"/>
+      <c r="C36" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="D36" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>146</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="D37" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>101</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="D38" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>100</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="D39" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>102</v>
+      </c>
+      <c r="C40" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="D40" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>119</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="D41" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>148</v>
+      </c>
+      <c r="C42" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="D42" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>107</v>
+      </c>
+      <c r="C43" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="D43" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>91</v>
+      </c>
+      <c r="C44" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="D44" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>105</v>
+      </c>
+      <c r="C45" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="D45" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>106</v>
+      </c>
+      <c r="C46" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="D46" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>103</v>
+      </c>
+      <c r="C47" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="D47" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>104</v>
+      </c>
+      <c r="C48" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="D48" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>108</v>
+      </c>
+      <c r="C49" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="D49" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>109</v>
+      </c>
+      <c r="C50" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="D50" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>110</v>
+      </c>
+      <c r="C51" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="D51" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>151</v>
+      </c>
+      <c r="C52" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="D52" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>124</v>
+      </c>
+      <c r="C53" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="D53" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>122</v>
+      </c>
+      <c r="C54" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="D54" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>111</v>
+      </c>
+      <c r="C55" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="D55" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>112</v>
+      </c>
+      <c r="C56" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="D56" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>113</v>
+      </c>
+      <c r="C57" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="D57" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>114</v>
+      </c>
+      <c r="C58" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="D58" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>115</v>
+      </c>
+      <c r="C59" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="D59" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>125</v>
+      </c>
+      <c r="C60" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="D60" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>116</v>
+      </c>
+      <c r="C61" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="D61" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>117</v>
+      </c>
+      <c r="C62" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="D62" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>128</v>
+      </c>
+      <c r="C63" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="D63" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>154</v>
+      </c>
+      <c r="C64" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="D64" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>121</v>
+      </c>
+      <c r="C65" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="D65" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>127</v>
+      </c>
+      <c r="C66" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="D66" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>152</v>
+      </c>
+      <c r="C67" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="D67" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>153</v>
+      </c>
+      <c r="C68" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="D68" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>126</v>
+      </c>
+      <c r="C69" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="D69" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>36</v>
+      </c>
+      <c r="C70" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="D70" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>31</v>
+      </c>
+      <c r="C71" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="D71" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>118</v>
+      </c>
+      <c r="C72" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="D72" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>35</v>
+      </c>
+      <c r="C73" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="D73" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>82</v>
+      </c>
+      <c r="C74" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="D74" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>34</v>
+      </c>
+      <c r="C75" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="D75" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>33</v>
+      </c>
+      <c r="C76" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="D76" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>156</v>
+      </c>
+      <c r="C77" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="D77" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>32</v>
+      </c>
+      <c r="C78" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="D78" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>79</v>
+      </c>
+      <c r="C79" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="D79" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>23</v>
+      </c>
+      <c r="C80" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="D80" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>158</v>
+      </c>
+      <c r="C81" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="D81" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>4</v>
+      </c>
+      <c r="C82" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="D82" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>159</v>
+      </c>
+      <c r="C83" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="D83" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>160</v>
+      </c>
+      <c r="C84" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="D84" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>21</v>
+      </c>
+      <c r="C85" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="D85" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>22</v>
+      </c>
+      <c r="C86" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="D86" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>20</v>
+      </c>
+      <c r="C87" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="D87" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>19</v>
+      </c>
+      <c r="C88" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="D88" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>18</v>
+      </c>
+      <c r="C89" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="D89" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>16</v>
+      </c>
+      <c r="C90" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="D90" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>17</v>
+      </c>
+      <c r="C91" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="D91" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>15</v>
+      </c>
+      <c r="C92" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="D92" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>14</v>
+      </c>
+      <c r="C93" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="D93" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>13</v>
+      </c>
+      <c r="C94" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="D94" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>12</v>
+      </c>
+      <c r="C95" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="D95" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>11</v>
+      </c>
+      <c r="C96" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="D96" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>10</v>
+      </c>
+      <c r="C97" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="D97" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>161</v>
+      </c>
+      <c r="C98" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="D98" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>123</v>
+      </c>
+      <c r="C99" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="D99" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>162</v>
+      </c>
+      <c r="C100" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="D100" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>163</v>
+      </c>
+      <c r="C101" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="D101" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>164</v>
+      </c>
+      <c r="C102" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="D102" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>120</v>
+      </c>
+      <c r="C103" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="D103" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>165</v>
+      </c>
+      <c r="C104" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="D104" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>78</v>
+      </c>
+      <c r="C105" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="D105" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>166</v>
+      </c>
+      <c r="C106" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="D106" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>169</v>
+      </c>
+      <c r="C107" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="D107" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>170</v>
+      </c>
+      <c r="C108" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="D108" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>37</v>
+      </c>
+      <c r="C109" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="D109" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>30</v>
+      </c>
+      <c r="C110" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="D110" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>172</v>
+      </c>
+      <c r="C111" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="D111" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>171</v>
+      </c>
+      <c r="C112" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="D112" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>71</v>
+      </c>
+      <c r="B113" s="3"/>
+      <c r="C113" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="D113" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>70</v>
+      </c>
+      <c r="B114" s="2"/>
+      <c r="C114" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="D114" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>72</v>
+      </c>
+      <c r="B115" s="3"/>
+      <c r="C115" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="D115" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>7</v>
+      </c>
+      <c r="B116" s="3"/>
+      <c r="C116" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="D116" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>69</v>
+      </c>
+      <c r="B117" s="3"/>
+      <c r="C117" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="D117" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>29</v>
+      </c>
+      <c r="C118" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="D118" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>24</v>
+      </c>
+      <c r="C119" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="D119" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>27</v>
+      </c>
+      <c r="B120" s="3"/>
+      <c r="C120" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="D120" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>174</v>
+      </c>
+      <c r="C121" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="D121" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>175</v>
+      </c>
+      <c r="C122" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="D122" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>81</v>
+      </c>
+      <c r="B123" s="2"/>
+      <c r="C123" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="D123" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>25</v>
+      </c>
+      <c r="C124" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="D124" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>26</v>
+      </c>
+      <c r="C125" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="D125" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>178</v>
+      </c>
+      <c r="C126" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="D126" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>179</v>
+      </c>
+      <c r="C127" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="D127" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>180</v>
+      </c>
+      <c r="C128" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="D128" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>181</v>
+      </c>
+      <c r="C129" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="D129" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>177</v>
+      </c>
+      <c r="C130" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="D130" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>182</v>
+      </c>
+      <c r="C131" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="D131" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>183</v>
+      </c>
+      <c r="C132" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="D132" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>184</v>
+      </c>
+      <c r="C133" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="D133" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>56</v>
+      </c>
+      <c r="C134" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="D134" t="s">
+        <v>141</v>
+      </c>
+      <c r="E134" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>50</v>
+      </c>
+      <c r="C135" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="D135" t="s">
+        <v>141</v>
+      </c>
+      <c r="E135" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>51</v>
+      </c>
+      <c r="C136" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="D136" t="s">
+        <v>141</v>
+      </c>
+      <c r="E136" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>47</v>
+      </c>
+      <c r="C137" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="D137" t="s">
+        <v>141</v>
+      </c>
+      <c r="E137" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>45</v>
+      </c>
+      <c r="C138" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="D138" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>44</v>
+      </c>
+      <c r="C139" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="D139" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>57</v>
+      </c>
+      <c r="C140" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="D140" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>58</v>
+      </c>
+      <c r="B141" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C141" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="D141" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>46</v>
+      </c>
+      <c r="C142" s="8" t="s">
+        <v>188</v>
+      </c>
+      <c r="D142" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>55</v>
+      </c>
+      <c r="C143" s="8" t="s">
+        <v>188</v>
+      </c>
+      <c r="D143" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>54</v>
+      </c>
+      <c r="C144" s="8" t="s">
+        <v>188</v>
+      </c>
+      <c r="D144" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>202</v>
+      </c>
+      <c r="C145" s="8" t="s">
+        <v>188</v>
+      </c>
+      <c r="D145" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>49</v>
+      </c>
+      <c r="C146" s="8" t="s">
+        <v>188</v>
+      </c>
+      <c r="D146" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>48</v>
+      </c>
+      <c r="C147" s="8" t="s">
+        <v>188</v>
+      </c>
+      <c r="D147" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>60</v>
+      </c>
+      <c r="C148" s="8" t="s">
+        <v>189</v>
+      </c>
+      <c r="D148" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>52</v>
+      </c>
+      <c r="C149" s="8" t="s">
+        <v>189</v>
+      </c>
+      <c r="D149" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>53</v>
+      </c>
+      <c r="C150" s="8" t="s">
+        <v>189</v>
+      </c>
+      <c r="D150" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>59</v>
+      </c>
+      <c r="C151" s="8" t="s">
+        <v>189</v>
+      </c>
+      <c r="D151" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>40</v>
+      </c>
+      <c r="C152" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="D152" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
+        <v>41</v>
+      </c>
+      <c r="C153" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="D153" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>42</v>
+      </c>
+      <c r="C154" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="D154" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>39</v>
+      </c>
+      <c r="C155" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="D155" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>38</v>
+      </c>
+      <c r="C156" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="D156" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>43</v>
+      </c>
+      <c r="C157" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="D157" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
+        <v>193</v>
+      </c>
+      <c r="C158" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="D158" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
+        <v>192</v>
+      </c>
+      <c r="C159" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="D159" t="s">
+        <v>141</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:G159">
+    <sortState ref="A2:G158">
+      <sortCondition ref="C1:C158"/>
+    </sortState>
+  </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="54.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>7</v>
+        <v>58</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A1:A19">
+  <sortState ref="A1:B4">
     <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -866,12 +2925,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection sqref="A1:B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -880,88 +2939,82 @@
     <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="B1" s="3"/>
-      <c r="C1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B2" s="3"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>75</v>
       </c>
       <c r="B3" s="3"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>76</v>
       </c>
-      <c r="B4" s="3"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B5" s="2"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>77</v>
-      </c>
-      <c r="B6" s="2"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
         <v>64</v>
       </c>
     </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B12" s="3"/>
+    </row>
   </sheetData>
-  <sortState ref="A1:A18">
+  <sortState ref="A1:B12">
     <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection sqref="A1:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -993,11 +3046,9 @@
       <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>73</v>
-      </c>
+      <c r="B4" s="3"/>
       <c r="C4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1006,7 +3057,7 @@
       </c>
       <c r="B5" s="3"/>
       <c r="C5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -1017,12 +3068,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1033,53 +3084,53 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B3" s="2"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B4" s="2"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B5" s="2"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B6" s="2"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B7" s="2"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B8" s="2"/>
     </row>
@@ -1091,12 +3142,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="R47" sqref="R47"/>
+      <selection sqref="A1:A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1106,14 +3157,14 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>97</v>
-      </c>
-      <c r="B1" s="2"/>
+        <v>91</v>
+      </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>92</v>
-      </c>
+        <v>105</v>
+      </c>
+      <c r="B2" s="3"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -1123,19 +3174,13 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="B4" s="3"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>104</v>
-      </c>
-      <c r="B5" s="3"/>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -1147,12 +3192,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection sqref="A1:B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1163,48 +3208,79 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>93</v>
-      </c>
-      <c r="B1" s="4"/>
+        <v>96</v>
+      </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>98</v>
-      </c>
-      <c r="B2" s="3"/>
+        <v>130</v>
+      </c>
+      <c r="B2" s="2"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>99</v>
-      </c>
-      <c r="B3" s="3"/>
+        <v>144</v>
+      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>96</v>
-      </c>
-      <c r="B4" s="3"/>
+        <v>92</v>
+      </c>
+      <c r="B4" s="4"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B5" s="3"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B6" s="3"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>95</v>
+      </c>
+      <c r="B8" s="3"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>94</v>
       </c>
-      <c r="B7" s="3"/>
+      <c r="B9" s="3"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>99</v>
+      </c>
+      <c r="B10" s="3"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>93</v>
+      </c>
+      <c r="B12" s="3"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>146</v>
+      </c>
     </row>
   </sheetData>
-  <sortState ref="A1:B8">
+  <sortState ref="A1:B13">
     <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1212,12 +3288,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection sqref="A1:A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1227,36 +3303,41 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B1" s="3"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B2" s="3"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B3" s="3"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B4" s="3"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>109</v>
+        <v>148</v>
       </c>
       <c r="B5" s="5"/>
     </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>107</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState ref="A1:A5">
+  <sortState ref="A1:A6">
     <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1264,7 +3345,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
@@ -1276,12 +3357,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection sqref="A1:A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1291,67 +3372,67 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B1" s="3"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B2" s="3"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B3" s="3"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>126</v>
+        <v>151</v>
       </c>
       <c r="B4" s="3"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>113</v>
+        <v>124</v>
       </c>
       <c r="B5" s="3"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
       <c r="B6" s="3"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B7" s="3"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B8" s="3"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B9" s="3"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B10" s="3"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -1362,12 +3443,12 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -1378,30 +3459,40 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>129</v>
+        <v>154</v>
       </c>
       <c r="B16" s="3"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="B17" s="3"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B18" s="3"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>132</v>
+        <v>152</v>
       </c>
       <c r="B19" s="3"/>
     </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>126</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState ref="A1:A14">
+  <sortState ref="A1:A21">
     <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1409,24 +3500,146 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>171</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A1:A6">
+    <sortCondition ref="A1"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B12"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="36.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B1" s="2"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>86</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A1:B11">
+    <sortCondition ref="A1"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection sqref="A1:A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1436,27 +3649,1481 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>124</v>
-      </c>
-      <c r="B1" s="2"/>
+        <v>161</v>
+      </c>
+      <c r="B1" s="3"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>127</v>
-      </c>
-      <c r="B2" s="3"/>
+        <v>123</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>166</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A14"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+      <selection sqref="A1:A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>160</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>184</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>192</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B158"/>
+  <sheetViews>
+    <sheetView topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="B78" sqref="B78"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="54.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>195</v>
+      </c>
+      <c r="B2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>96</v>
+      </c>
+      <c r="B8" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>129</v>
+      </c>
+      <c r="B9" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>130</v>
+      </c>
+      <c r="B10" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>60</v>
+      </c>
+      <c r="B14" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>43</v>
+      </c>
+      <c r="B17" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>144</v>
+      </c>
+      <c r="B18" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>91</v>
+      </c>
+      <c r="B19" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>108</v>
+      </c>
+      <c r="B20" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>109</v>
+      </c>
+      <c r="B21" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>110</v>
+      </c>
+      <c r="B22" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>151</v>
+      </c>
+      <c r="B23" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>45</v>
+      </c>
+      <c r="B24" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>44</v>
+      </c>
+      <c r="B25" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>57</v>
+      </c>
+      <c r="B27" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>58</v>
+      </c>
+      <c r="B28" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>31</v>
+      </c>
+      <c r="B29" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>178</v>
+      </c>
+      <c r="B30" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>92</v>
+      </c>
+      <c r="B31" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>101</v>
+      </c>
+      <c r="B32" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>77</v>
+      </c>
+      <c r="B33" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>100</v>
+      </c>
+      <c r="B34" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>24</v>
+      </c>
+      <c r="B35" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>74</v>
+      </c>
+      <c r="B36" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>206</v>
+      </c>
+      <c r="B37" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>9</v>
+      </c>
+      <c r="B38" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>56</v>
+      </c>
+      <c r="B39" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>161</v>
+      </c>
+      <c r="B40" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>124</v>
+      </c>
+      <c r="B41" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>123</v>
+      </c>
+      <c r="B42" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>80</v>
+      </c>
+      <c r="B43" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>71</v>
+      </c>
+      <c r="B44" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>70</v>
+      </c>
+      <c r="B45" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>179</v>
+      </c>
+      <c r="B46" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>102</v>
+      </c>
+      <c r="B47" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>97</v>
+      </c>
+      <c r="B48" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>98</v>
+      </c>
+      <c r="B49" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>27</v>
+      </c>
+      <c r="B50" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>180</v>
+      </c>
+      <c r="B51" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>122</v>
+      </c>
+      <c r="B52" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>21</v>
+      </c>
+      <c r="B53" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>22</v>
+      </c>
+      <c r="B54" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>181</v>
+      </c>
+      <c r="B55" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>118</v>
+      </c>
+      <c r="B56" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>145</v>
+      </c>
+      <c r="B57" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>35</v>
+      </c>
+      <c r="B58" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>174</v>
+      </c>
+      <c r="B59" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>82</v>
+      </c>
+      <c r="B60" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>162</v>
+      </c>
+      <c r="B61" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>34</v>
+      </c>
+      <c r="B62" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>201</v>
+      </c>
+      <c r="B63" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>55</v>
+      </c>
+      <c r="B64" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>95</v>
+      </c>
+      <c r="B65" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>94</v>
+      </c>
+      <c r="B66" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>73</v>
+      </c>
+      <c r="B67" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>199</v>
+      </c>
+      <c r="B68" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>20</v>
+      </c>
+      <c r="B69" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>8</v>
+      </c>
+      <c r="B70" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>19</v>
+      </c>
+      <c r="B71" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>81</v>
+      </c>
+      <c r="B72" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>54</v>
+      </c>
+      <c r="B73" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>105</v>
+      </c>
+      <c r="B74" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>200</v>
+      </c>
+      <c r="B75" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>158</v>
+      </c>
+      <c r="B76" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>163</v>
+      </c>
+      <c r="B77" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>197</v>
+      </c>
+      <c r="B78" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>198</v>
+      </c>
+      <c r="B79" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>164</v>
+      </c>
+      <c r="B80" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>113</v>
+      </c>
+      <c r="B81" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>99</v>
+      </c>
+      <c r="B82" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>18</v>
+      </c>
+      <c r="B83" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>5</v>
+      </c>
+      <c r="B84" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>6</v>
+      </c>
+      <c r="B85" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>52</v>
+      </c>
+      <c r="B86" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>53</v>
+      </c>
+      <c r="B87" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>120</v>
+      </c>
+      <c r="B88" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>114</v>
+      </c>
+      <c r="B89" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>115</v>
+      </c>
+      <c r="B90" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>4</v>
+      </c>
+      <c r="B91" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>50</v>
+      </c>
+      <c r="B92" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>51</v>
+      </c>
+      <c r="B93" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>76</v>
+      </c>
+      <c r="B94" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>202</v>
+      </c>
+      <c r="B95" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>119</v>
+      </c>
+      <c r="B96" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>2</v>
+      </c>
+      <c r="B97" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>3</v>
+      </c>
+      <c r="B98" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>16</v>
+      </c>
+      <c r="B99" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>17</v>
+      </c>
+      <c r="B100" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>1</v>
+      </c>
+      <c r="B101" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>15</v>
+      </c>
+      <c r="B102" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>14</v>
+      </c>
+      <c r="B103" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>125</v>
+      </c>
+      <c r="B104" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>165</v>
+      </c>
+      <c r="B105" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>13</v>
+      </c>
+      <c r="B106" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>12</v>
+      </c>
+      <c r="B107" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>205</v>
+      </c>
+      <c r="B108" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>182</v>
+      </c>
+      <c r="B109" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>0</v>
+      </c>
+      <c r="B110" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>11</v>
+      </c>
+      <c r="B111" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>49</v>
+      </c>
+      <c r="B112" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>148</v>
+      </c>
+      <c r="B113" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>65</v>
+      </c>
+      <c r="B114" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>63</v>
+      </c>
+      <c r="B115" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>66</v>
+      </c>
+      <c r="B116" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>67</v>
+      </c>
+      <c r="B117" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>62</v>
+      </c>
+      <c r="B118" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>142</v>
+      </c>
+      <c r="B119" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>25</v>
+      </c>
+      <c r="B120" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>78</v>
+      </c>
+      <c r="B121" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>204</v>
+      </c>
+      <c r="B122" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>7</v>
+      </c>
+      <c r="B123" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>69</v>
+      </c>
+      <c r="B124" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>85</v>
+      </c>
+      <c r="B125" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>86</v>
+      </c>
+      <c r="B126" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>64</v>
+      </c>
+      <c r="B127" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>194</v>
+      </c>
+      <c r="B128" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>116</v>
+      </c>
+      <c r="B129" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>117</v>
+      </c>
+      <c r="B130" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>196</v>
+      </c>
+      <c r="B131" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>128</v>
+      </c>
+      <c r="B132" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>59</v>
+      </c>
+      <c r="B133" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>154</v>
+      </c>
+      <c r="B134" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>10</v>
+      </c>
+      <c r="B135" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>48</v>
+      </c>
+      <c r="B136" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>183</v>
+      </c>
+      <c r="B137" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>28</v>
+      </c>
+      <c r="B138" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>106</v>
+      </c>
+      <c r="B139" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>30</v>
+      </c>
+      <c r="B140" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>172</v>
+      </c>
+      <c r="B141" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>171</v>
+      </c>
+      <c r="B142" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>93</v>
+      </c>
+      <c r="B143" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>121</v>
+      </c>
+      <c r="B144" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>103</v>
+      </c>
+      <c r="B145" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>104</v>
+      </c>
+      <c r="B146" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>160</v>
+      </c>
+      <c r="B147" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>203</v>
+      </c>
+      <c r="B148" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>26</v>
+      </c>
+      <c r="B149" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>32</v>
+      </c>
+      <c r="B150" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>47</v>
+      </c>
+      <c r="B151" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>107</v>
+      </c>
+      <c r="B152" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
+        <v>146</v>
+      </c>
+      <c r="B153" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>127</v>
+      </c>
+      <c r="B154" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>152</v>
+      </c>
+      <c r="B155" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>153</v>
+      </c>
+      <c r="B156" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>126</v>
+      </c>
+      <c r="B157" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
+        <v>184</v>
+      </c>
+      <c r="B158" t="s">
+        <v>184</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A1:A160">
+    <sortCondition ref="A114"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:A14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1464,11 +5131,6 @@
     <col min="1" max="1" width="34.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>23</v>
-      </c>
-    </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>21</v>
@@ -1542,12 +5204,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1573,44 +5235,44 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>174</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>175</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>26</v>
-      </c>
+        <v>81</v>
+      </c>
+      <c r="B6" s="2"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>133</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>82</v>
-      </c>
-      <c r="B8" s="2"/>
+        <v>26</v>
+      </c>
     </row>
   </sheetData>
-  <sortState ref="A1:A6">
+  <sortState ref="A1:B10">
     <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection sqref="A1:A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1620,71 +5282,65 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B1" s="3"/>
+        <v>36</v>
+      </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>118</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>122</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>156</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>37</v>
-      </c>
-      <c r="B10" s="2"/>
+        <v>32</v>
+      </c>
+      <c r="B9" s="3"/>
     </row>
   </sheetData>
   <sortState ref="A1:A10">
-    <sortCondition descending="1" ref="A1"/>
+    <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+      <selection sqref="A1:A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1722,12 +5378,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C5"/>
+      <selection sqref="A1:A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1779,12 +5435,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1807,9 +5463,7 @@
       <c r="A3" t="s">
         <v>53</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>107</v>
-      </c>
+      <c r="B3" s="2"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -1825,12 +5479,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1858,61 +5512,23 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>49</v>
+        <v>202</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>48</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="54.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="44" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>58</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-  </sheetData>
-  <sortState ref="A1:B4">
+  <sortState ref="A1:A6">
     <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>